<commit_message>
update newmutdata til 2016
</commit_message>
<xml_diff>
--- a/Newrifmutdata/Newmutdata/newpaper.xlsx
+++ b/Newrifmutdata/Newmutdata/newpaper.xlsx
@@ -5588,8 +5588,8 @@
   <sheetPr/>
   <dimension ref="A1:Z180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" topLeftCell="I7" workbookViewId="0">
+      <selection activeCell="Z29" sqref="Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4"/>
@@ -6022,7 +6022,7 @@
       <c r="E9">
         <v>2021</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>90</v>
       </c>
       <c r="H9" t="s">
@@ -6069,7 +6069,7 @@
       <c r="E10">
         <v>2020</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="3" t="s">
         <v>98</v>
       </c>
       <c r="H10" t="s">
@@ -6100,7 +6100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:26">
       <c r="A11" t="s">
         <v>103</v>
       </c>
@@ -6143,8 +6143,11 @@
       <c r="W11" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="12" spans="1:23">
+      <c r="Z11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -6187,8 +6190,11 @@
       <c r="W12" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="13" spans="1:23">
+      <c r="Z12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -6231,8 +6237,11 @@
       <c r="W13" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="14" spans="1:23">
+      <c r="Z13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
       <c r="A14" t="s">
         <v>129</v>
       </c>
@@ -6248,7 +6257,7 @@
       <c r="E14">
         <v>2018</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="1" t="s">
         <v>133</v>
       </c>
       <c r="H14" t="s">
@@ -6275,8 +6284,11 @@
       <c r="W14" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="15" spans="1:23">
+      <c r="Z14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
       <c r="A15" t="s">
         <v>138</v>
       </c>
@@ -6292,7 +6304,7 @@
       <c r="E15">
         <v>2018</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="1" t="s">
         <v>141</v>
       </c>
       <c r="H15" t="s">
@@ -6319,8 +6331,11 @@
       <c r="W15" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="16" spans="1:23">
+      <c r="Z15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
       <c r="A16" t="s">
         <v>146</v>
       </c>
@@ -6336,7 +6351,7 @@
       <c r="E16">
         <v>2018</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="1" t="s">
         <v>150</v>
       </c>
       <c r="H16" t="s">
@@ -6363,8 +6378,11 @@
       <c r="W16" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="17" spans="1:23">
+      <c r="Z16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
       <c r="A17" t="s">
         <v>155</v>
       </c>
@@ -6380,7 +6398,7 @@
       <c r="E17">
         <v>2017</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="1" t="s">
         <v>159</v>
       </c>
       <c r="H17" t="s">
@@ -6407,8 +6425,11 @@
       <c r="W17" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="18" spans="1:23">
+      <c r="Z17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
       <c r="A18" t="s">
         <v>164</v>
       </c>
@@ -6424,7 +6445,7 @@
       <c r="E18">
         <v>2016</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="1" t="s">
         <v>168</v>
       </c>
       <c r="H18" t="s">
@@ -6451,8 +6472,11 @@
       <c r="W18" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="19" spans="1:23">
+      <c r="Z18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
       <c r="A19" t="s">
         <v>173</v>
       </c>
@@ -6468,7 +6492,7 @@
       <c r="E19">
         <v>2016</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="1" t="s">
         <v>177</v>
       </c>
       <c r="H19" t="s">
@@ -6495,8 +6519,11 @@
       <c r="W19" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="20" spans="1:23">
+      <c r="Z19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
       <c r="A20" t="s">
         <v>182</v>
       </c>
@@ -6512,7 +6539,7 @@
       <c r="E20">
         <v>2016</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="1" t="s">
         <v>185</v>
       </c>
       <c r="H20" t="s">
@@ -6539,8 +6566,11 @@
       <c r="W20" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="21" spans="1:23">
+      <c r="Z20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26">
       <c r="A21" t="s">
         <v>190</v>
       </c>
@@ -6556,7 +6586,7 @@
       <c r="E21">
         <v>2016</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="1" t="s">
         <v>194</v>
       </c>
       <c r="H21" t="s">
@@ -6583,8 +6613,11 @@
       <c r="W21" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="22" spans="1:23">
+      <c r="Z21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26">
       <c r="A22" t="s">
         <v>199</v>
       </c>
@@ -6600,7 +6633,7 @@
       <c r="E22">
         <v>2016</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="1" t="s">
         <v>203</v>
       </c>
       <c r="H22" t="s">
@@ -6626,6 +6659,9 @@
       </c>
       <c r="W22" t="s">
         <v>207</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:23">

</xml_diff>